<commit_message>
Added Category and Item Functionality & default Padrone admin & welcomeUser/Customer 'menu' based on available categories in database
</commit_message>
<xml_diff>
--- a/doc/base/Statusbericht.xlsx
+++ b/doc/base/Statusbericht.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Nils:</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>LoginDB</t>
+  </si>
+  <si>
+    <t>addUser nonEmtpy Validation added and some(user) handling from getUser function implemented</t>
   </si>
 </sst>
 </file>
@@ -380,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:C5"/>
+  <dimension ref="A4:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,6 +410,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42692</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>